<commit_message>
Add test Megacom number
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">transport_osh</t>
   </si>
   <si>
-    <t xml:space="preserve">FoLdEr</t>
+    <t xml:space="preserve">Transport_Osh</t>
   </si>
   <si>
     <t xml:space="preserve">260_AC</t>
@@ -526,7 +526,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -555,7 +555,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -565,6 +565,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -610,7 +614,7 @@
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.43"/>
@@ -666,7 +670,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="10" t="s">
         <v>11</v>
       </c>
     </row>
@@ -677,7 +681,7 @@
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -693,7 +697,7 @@
       <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -709,7 +713,7 @@
       <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -725,7 +729,7 @@
       <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -741,7 +745,7 @@
       <c r="B8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -757,7 +761,7 @@
       <c r="B9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -773,7 +777,7 @@
       <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -789,7 +793,7 @@
       <c r="B11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -805,7 +809,7 @@
       <c r="B12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -821,7 +825,7 @@
       <c r="B13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -837,7 +841,7 @@
       <c r="B14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -853,7 +857,7 @@
       <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -885,7 +889,7 @@
       <c r="B17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -901,7 +905,7 @@
       <c r="B18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -917,7 +921,7 @@
       <c r="B19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="11" t="s">
         <v>43</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -933,7 +937,7 @@
       <c r="B20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="11" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -949,7 +953,7 @@
       <c r="B21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="11" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -965,7 +969,7 @@
       <c r="B22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="11" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -997,7 +1001,7 @@
       <c r="B24" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="11" t="s">
         <v>53</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -1010,10 +1014,10 @@
       <c r="A25" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="11" t="s">
         <v>55</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -1026,10 +1030,10 @@
       <c r="A26" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="11" t="s">
         <v>57</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -1042,10 +1046,10 @@
       <c r="A27" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="11" t="s">
         <v>59</v>
       </c>
       <c r="D27" s="5" t="s">
@@ -1058,10 +1062,10 @@
       <c r="A28" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="11" t="s">
         <v>61</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -1074,10 +1078,10 @@
       <c r="A29" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="11" t="s">
         <v>63</v>
       </c>
       <c r="D29" s="5" t="s">
@@ -1090,10 +1094,10 @@
       <c r="A30" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="11" t="s">
         <v>65</v>
       </c>
       <c r="D30" s="5" t="s">
@@ -1106,7 +1110,7 @@
       <c r="A31" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="12" t="s">
         <v>66</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -1122,10 +1126,10 @@
       <c r="A32" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="11" t="s">
         <v>69</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -1138,10 +1142,10 @@
       <c r="A33" s="6" t="n">
         <v>31</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="11" t="s">
         <v>71</v>
       </c>
       <c r="D33" s="5" t="s">
@@ -1154,10 +1158,10 @@
       <c r="A34" s="6" t="n">
         <v>32</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D34" s="5" t="s">
@@ -1170,10 +1174,10 @@
       <c r="A35" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="14" t="s">
         <v>75</v>
       </c>
       <c r="D35" s="5" t="s">
@@ -1186,10 +1190,10 @@
       <c r="A36" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="14" t="s">
         <v>77</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -1202,10 +1206,10 @@
       <c r="A37" s="6" t="n">
         <v>35</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="14" t="s">
         <v>79</v>
       </c>
       <c r="D37" s="5" t="s">
@@ -1218,10 +1222,10 @@
       <c r="A38" s="6" t="n">
         <v>36</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="14" t="s">
         <v>81</v>
       </c>
       <c r="D38" s="5" t="s">
@@ -1234,10 +1238,10 @@
       <c r="A39" s="6" t="n">
         <v>37</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="14" t="s">
         <v>83</v>
       </c>
       <c r="D39" s="5" t="s">
@@ -1250,10 +1254,10 @@
       <c r="A40" s="6" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="14" t="s">
         <v>85</v>
       </c>
       <c r="D40" s="5" t="s">
@@ -1266,10 +1270,10 @@
       <c r="A41" s="6" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="14" t="s">
         <v>87</v>
       </c>
       <c r="D41" s="5" t="s">
@@ -1282,10 +1286,10 @@
       <c r="A42" s="6" t="n">
         <v>40</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="14" t="s">
         <v>89</v>
       </c>
       <c r="D42" s="5" t="s">
@@ -1298,10 +1302,10 @@
       <c r="A43" s="6" t="n">
         <v>41</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="14" t="s">
         <v>91</v>
       </c>
       <c r="D43" s="5" t="s">
@@ -1317,7 +1321,7 @@
       <c r="B44" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="14" t="s">
         <v>93</v>
       </c>
       <c r="D44" s="5" t="s">
@@ -1330,10 +1334,10 @@
       <c r="A45" s="6" t="n">
         <v>43</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="14" t="s">
         <v>95</v>
       </c>
       <c r="D45" s="5" t="s">
@@ -1346,10 +1350,10 @@
       <c r="A46" s="6" t="n">
         <v>44</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="14" t="s">
         <v>97</v>
       </c>
       <c r="D46" s="5" t="s">
@@ -1362,10 +1366,10 @@
       <c r="A47" s="6" t="n">
         <v>45</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="14" t="s">
         <v>99</v>
       </c>
       <c r="D47" s="5" t="s">
@@ -1378,10 +1382,10 @@
       <c r="A48" s="6" t="n">
         <v>46</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="14" t="s">
         <v>101</v>
       </c>
       <c r="D48" s="5" t="s">
@@ -1394,10 +1398,10 @@
       <c r="A49" s="6" t="n">
         <v>47</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="14" t="s">
         <v>103</v>
       </c>
       <c r="D49" s="5" t="s">
@@ -1410,10 +1414,10 @@
       <c r="A50" s="6" t="n">
         <v>48</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="14" t="s">
         <v>105</v>
       </c>
       <c r="D50" s="5" t="s">
@@ -1426,10 +1430,10 @@
       <c r="A51" s="6" t="n">
         <v>49</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="14" t="s">
         <v>107</v>
       </c>
       <c r="D51" s="5" t="s">
@@ -1442,10 +1446,10 @@
       <c r="A52" s="6" t="n">
         <v>50</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="14" t="s">
         <v>109</v>
       </c>
       <c r="D52" s="5" t="s">
@@ -1458,10 +1462,10 @@
       <c r="A53" s="6" t="n">
         <v>51</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="14" t="s">
         <v>111</v>
       </c>
       <c r="D53" s="5" t="s">
@@ -1474,10 +1478,10 @@
       <c r="A54" s="6" t="n">
         <v>52</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="14" t="s">
         <v>113</v>
       </c>
       <c r="D54" s="5" t="s">
@@ -1490,10 +1494,10 @@
       <c r="A55" s="6" t="n">
         <v>53</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D55" s="5" t="s">
@@ -1506,10 +1510,10 @@
       <c r="A56" s="6" t="n">
         <v>54</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="14" t="s">
         <v>117</v>
       </c>
       <c r="D56" s="5" t="s">
@@ -1522,10 +1526,10 @@
       <c r="A57" s="6" t="n">
         <v>55</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C57" s="14" t="s">
         <v>119</v>
       </c>
       <c r="D57" s="5" t="s">
@@ -1538,10 +1542,10 @@
       <c r="A58" s="6" t="n">
         <v>56</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C58" s="14" t="s">
         <v>121</v>
       </c>
       <c r="D58" s="5" t="s">
@@ -1554,10 +1558,10 @@
       <c r="A59" s="6" t="n">
         <v>57</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="14" t="s">
         <v>123</v>
       </c>
       <c r="D59" s="5" t="s">
@@ -1570,10 +1574,10 @@
       <c r="A60" s="6" t="n">
         <v>58</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="14" t="s">
         <v>125</v>
       </c>
       <c r="D60" s="5" t="s">
@@ -1586,10 +1590,10 @@
       <c r="A61" s="6" t="n">
         <v>59</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="14" t="s">
         <v>127</v>
       </c>
       <c r="D61" s="5" t="s">

</xml_diff>